<commit_message>
Added data point from MPLS.
</commit_message>
<xml_diff>
--- a/Data/EO Timeline.xlsx
+++ b/Data/EO Timeline.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c42bfdeb173e779/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c42bfdeb173e779/Desktop/project-1/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="8_{614F6411-227F-44C7-9D39-672C4347A972}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{041A6109-1F08-4962-883F-1BE72D3D7A1A}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="8_{614F6411-227F-44C7-9D39-672C4347A972}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{812B0FCB-C278-44E0-BE10-36F28611E2D0}"/>
   <bookViews>
-    <workbookView xWindow="5260" yWindow="5640" windowWidth="16200" windowHeight="10060" xr2:uid="{38F3180D-66CA-43AD-B83D-C739AF1A2AA6}"/>
+    <workbookView xWindow="5260" yWindow="3740" windowWidth="16200" windowHeight="10060" xr2:uid="{38F3180D-66CA-43AD-B83D-C739AF1A2AA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>EO #</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Nice Ride season end</t>
+  </si>
+  <si>
+    <t>Mayor Frey orders indoor dining closed 8/1</t>
   </si>
 </sst>
 </file>
@@ -539,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212559F6-5F84-43C0-9C31-2B505C600D68}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -793,50 +796,58 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>44055</v>
-      </c>
-      <c r="B23" t="s">
-        <v>42</v>
+        <v>44041</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
-        <v>44069</v>
+        <v>44055</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>44082</v>
+        <v>44069</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
-        <v>44139</v>
+        <v>44082</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
+        <v>44139</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
         <v>44145</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>46</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Figuring out how to build timeline plot.
</commit_message>
<xml_diff>
--- a/Data/EO Timeline.xlsx
+++ b/Data/EO Timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c42bfdeb173e779/Desktop/project-1/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="8_{614F6411-227F-44C7-9D39-672C4347A972}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{812B0FCB-C278-44E0-BE10-36F28611E2D0}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="8_{614F6411-227F-44C7-9D39-672C4347A972}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AC8CE738-CA27-4B84-AA48-DF2728CA4C57}"/>
   <bookViews>
-    <workbookView xWindow="5260" yWindow="3740" windowWidth="16200" windowHeight="10060" xr2:uid="{38F3180D-66CA-43AD-B83D-C739AF1A2AA6}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="16200" windowHeight="10060" xr2:uid="{38F3180D-66CA-43AD-B83D-C739AF1A2AA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>EO #</t>
   </si>
@@ -190,6 +190,15 @@
   </si>
   <si>
     <t>Mayor Frey orders indoor dining closed 8/1</t>
+  </si>
+  <si>
+    <t>George Floyd murdered</t>
+  </si>
+  <si>
+    <t>Protests begin</t>
+  </si>
+  <si>
+    <t>National Guard Activated</t>
   </si>
 </sst>
 </file>
@@ -542,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{212559F6-5F84-43C0-9C31-2B505C600D68}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -752,102 +761,126 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>43978</v>
-      </c>
-      <c r="B19" t="s">
-        <v>35</v>
+        <v>43976</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <v>43987</v>
-      </c>
-      <c r="B20" t="s">
-        <v>37</v>
+        <v>43977</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
-        <v>43994</v>
+        <v>43978</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
-        <v>44025</v>
-      </c>
-      <c r="B22" t="s">
-        <v>41</v>
+        <v>43979</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>44041</v>
+        <v>43987</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
-        <v>44055</v>
+        <v>43994</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>44069</v>
+        <v>44025</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
-        <v>44082</v>
+        <v>44041</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
-        <v>44139</v>
+        <v>44055</v>
+      </c>
+      <c r="B27" t="s">
+        <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
+        <v>44069</v>
+      </c>
+      <c r="B28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>44082</v>
+      </c>
+      <c r="C29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>44139</v>
+      </c>
+      <c r="C30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
         <v>44145</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B31" t="s">
         <v>46</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C31" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>